<commit_message>
Update .gitignore to include demo files; add agent.py and testing.py; enhance email content generation
</commit_message>
<xml_diff>
--- a/demo.xlsx
+++ b/demo.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\XZNON\cccc\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\XZNON\cccc\Desktop\emailing-agent\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A8A6FCA2-2D16-4D99-9710-3FB94119B034}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89FDDC53-8D50-4CBF-95C7-37D6ECC5BDDD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15960" xr2:uid="{0E578D8E-500C-4576-8606-43F7162E9D48}"/>
   </bookViews>
@@ -52,9 +52,6 @@
     <t>Akanksha Puri</t>
   </si>
   <si>
-    <t>akanksha.puri@sourcefuse.com</t>
-  </si>
-  <si>
     <t>Associate Director HR</t>
   </si>
   <si>
@@ -64,21 +61,9 @@
     <t>Akanksha Sogani</t>
   </si>
   <si>
-    <t>akanksha.sogani@perennialsys.com</t>
-  </si>
-  <si>
-    <t>Head HR</t>
-  </si>
-  <si>
-    <t>Perennial Systems</t>
-  </si>
-  <si>
     <t>Akhil Jogiparthi</t>
   </si>
   <si>
-    <t>akhil@ibhubs.co</t>
-  </si>
-  <si>
     <t>Vice President - Talent Accelerator</t>
   </si>
   <si>
@@ -88,23 +73,46 @@
     <t>Akhila Chandan</t>
   </si>
   <si>
-    <t>akhila@estuate.com</t>
-  </si>
-  <si>
     <t>Associate Vice President Human Resources</t>
   </si>
   <si>
     <t>Estuate,</t>
+  </si>
+  <si>
+    <t>shivaliksingh09@gmail.com</t>
+  </si>
+  <si>
+    <t>yashashviagnihotri007@gmail.com</t>
+  </si>
+  <si>
+    <t>Penis enlargement solutions</t>
+  </si>
+  <si>
+    <t>head simp</t>
+  </si>
+  <si>
+    <t>shivaliksingh39@gmail.com</t>
+  </si>
+  <si>
+    <t>shivaliksinghsolanki@gmail.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -127,16 +135,21 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -452,7 +465,7 @@
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -488,14 +501,14 @@
       <c r="B2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="E2" s="1" t="s">
         <v>7</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -503,16 +516,16 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>16</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -520,16 +533,16 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>14</v>
+        <v>9</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>20</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -537,19 +550,25 @@
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>18</v>
+        <v>12</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>15</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C2" r:id="rId1" xr:uid="{A6722D0B-CBD5-4FF0-A2C8-9A8D7D83A949}"/>
+    <hyperlink ref="C3" r:id="rId2" xr:uid="{7CE2DE65-E1DF-42B4-8342-12F59C2DA9B9}"/>
+    <hyperlink ref="C4" r:id="rId3" xr:uid="{4EB9984B-B364-4FC2-AB50-CC958F83B4A4}"/>
+    <hyperlink ref="C5" r:id="rId4" xr:uid="{070D79DA-B37A-472E-99F8-0E02C60E6BD2}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>